<commit_message>
Cập nhật ứng dụng
</commit_message>
<xml_diff>
--- a/US_dialog.xlsx
+++ b/US_dialog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndmnh\Desktop\Lesson\Lesson Online\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndmnh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF526C40-218B-459A-B9E1-157F0BFCBBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C7E7598-D92D-4EA4-9948-16F5A2E3E65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,18 +39,12 @@
     <t>Bạn đến từ đâu?</t>
   </si>
   <si>
-    <t>I’m from New York.</t>
-  </si>
-  <si>
     <t>Tôi đến từ New York.</t>
   </si>
   <si>
     <t>Bạn làm nghề gì?</t>
   </si>
   <si>
-    <t>I’m a teacher.</t>
-  </si>
-  <si>
     <t>Tôi là giáo viên.</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>Mấy giờ rồi?</t>
   </si>
   <si>
-    <t>It’s 3 PM.</t>
-  </si>
-  <si>
     <t>Question_IPA</t>
   </si>
   <si>
@@ -234,9 +225,6 @@
     <t>Tiền tip đã bao gồm chưa?</t>
   </si>
   <si>
-    <t>No, it’s separate.</t>
-  </si>
-  <si>
     <t>/noʊ, ɪts ˈsɛprɪt/</t>
   </si>
   <si>
@@ -261,9 +249,6 @@
     <t>Có, chúng tôi có!</t>
   </si>
   <si>
-    <t>How’s it going?</t>
-  </si>
-  <si>
     <t>/haʊz ɪt ˈɡoʊɪŋ?/</t>
   </si>
   <si>
@@ -279,9 +264,6 @@
     <t>Khá ổn!</t>
   </si>
   <si>
-    <t>What’s up?</t>
-  </si>
-  <si>
     <t>/wʌt's ʌp?/</t>
   </si>
   <si>
@@ -342,9 +324,6 @@
     <t>Bạn có thời gian nói chuyện không?</t>
   </si>
   <si>
-    <t>Yeah, what’s up?</t>
-  </si>
-  <si>
     <t>/jæ, wʌts ʌp?/</t>
   </si>
   <si>
@@ -381,9 +360,6 @@
     <t>Bạn có thích ở đây không?</t>
   </si>
   <si>
-    <t>Yeah, it’s nice!</t>
-  </si>
-  <si>
     <t>/jæ, ɪts naɪs!/</t>
   </si>
   <si>
@@ -426,9 +402,6 @@
     <t>Cái này bao nhiêu tiền?</t>
   </si>
   <si>
-    <t>It’s $25.99.</t>
-  </si>
-  <si>
     <t>/ɪts ˈtwɛnti faɪv ˌnaɪnti naɪn/</t>
   </si>
   <si>
@@ -507,9 +480,6 @@
     <t>Không, nhưng tuần sau sẽ giảm giá.</t>
   </si>
   <si>
-    <t>Can I return this if it doesn’t fit?</t>
-  </si>
-  <si>
     <t>/kæn aɪ rɪˈtɜrn ðɪs ɪf ɪt ˈdʌzənt fɪt?/</t>
   </si>
   <si>
@@ -555,9 +525,6 @@
     <t>Tất nhiên! Đây của bạn.</t>
   </si>
   <si>
-    <t>What’s your return policy?</t>
-  </si>
-  <si>
     <t>/wʌts jʊr rɪˈtɜrn ˈpɑləsi?/</t>
   </si>
   <si>
@@ -582,9 +549,6 @@
     <t>Khách sạn gần nhất ở đâu?</t>
   </si>
   <si>
-    <t>It’s two blocks away.</t>
-  </si>
-  <si>
     <t>/ɪts tu blɑks əˈweɪ/</t>
   </si>
   <si>
@@ -609,9 +573,6 @@
     <t>Bạn có thể đi taxi hoặc xe buýt.</t>
   </si>
   <si>
-    <t>What’s the best way to get around?</t>
-  </si>
-  <si>
     <t>/wʌts ðə bɛst weɪ tu ɡɛt əˈraʊnd?/</t>
   </si>
   <si>
@@ -726,9 +687,6 @@
     <t>Phí vào cửa là bao nhiêu?</t>
   </si>
   <si>
-    <t>It’s $10 per person.</t>
-  </si>
-  <si>
     <t>/ɪts tɛn dɑlərz pɜr ˈpɝːsən/</t>
   </si>
   <si>
@@ -762,9 +720,6 @@
     <t>Bạn có thể giới thiệu về mình không?</t>
   </si>
   <si>
-    <t>Sure! I’m Alex, a project manager.</t>
-  </si>
-  <si>
     <t>/ʃʊr! aɪm ˈæləks, ə ˈprɑʤɛkt ˈmænɪʤər/</t>
   </si>
   <si>
@@ -798,9 +753,6 @@
     <t>Hạn chót của dự án này là khi nào?</t>
   </si>
   <si>
-    <t>It’s due next Friday.</t>
-  </si>
-  <si>
     <t>/ɪts du nɛkst ˈfraɪdeɪ/</t>
   </si>
   <si>
@@ -834,9 +786,6 @@
     <t>Tôi nên báo cáo cho ai?</t>
   </si>
   <si>
-    <t>You’ll report to the department manager.</t>
-  </si>
-  <si>
     <t>/jul rɪˈpɔrt tu ðə dɪˈpɑrtmənt ˈmænɪʤər/</t>
   </si>
   <si>
@@ -852,9 +801,6 @@
     <t>Tôi có thể truy cập tài liệu bằng cách nào?</t>
   </si>
   <si>
-    <t>They’re on the company’s shared drive.</t>
-  </si>
-  <si>
     <t>/ðeɪr ɑn ðə ˈkʌmpəniʃɛrd draɪv/</t>
   </si>
   <si>
@@ -879,9 +825,6 @@
     <t>Có, vậy thì tốt quá!</t>
   </si>
   <si>
-    <t>What’s the next step in this process?</t>
-  </si>
-  <si>
     <t>/wʌts ðə nɛkst stɛp ɪn ðɪs ˈprɑsɛs?/</t>
   </si>
   <si>
@@ -906,18 +849,12 @@
     <t>Bạn có thể gửi tôi báo cáo không?</t>
   </si>
   <si>
-    <t>Sure, I’ll email it to you now.</t>
-  </si>
-  <si>
     <t>/ʃʊr, aɪl ˈimeɪl ɪt tu ju naʊ/</t>
   </si>
   <si>
     <t>Được, tôi sẽ gửi email ngay bây giờ.</t>
   </si>
   <si>
-    <t>How was the client’s feedback?</t>
-  </si>
-  <si>
     <t>/haʊ wəz ðə ˈklaɪənts ˈfidˌbæk?/</t>
   </si>
   <si>
@@ -999,9 +936,6 @@
     <t>/kæn aɪ ɡɛt ðə ʧɛk, pliz?/</t>
   </si>
   <si>
-    <t>Of course! I’ll bring it right away.</t>
-  </si>
-  <si>
     <t>/ʌv kɔrs! aɪl brɪŋ ɪt raɪt əˈweɪ/</t>
   </si>
   <si>
@@ -1023,9 +957,6 @@
     <t>/kæn aɪ ɡɛt ə tu-ɡoʊ bɑks?/</t>
   </si>
   <si>
-    <t>Sure! I’ll bring one for you.</t>
-  </si>
-  <si>
     <t>/ʃʊr! aɪl brɪŋ wʌn fɔr ju/</t>
   </si>
   <si>
@@ -1041,9 +972,6 @@
     <t>Ở đây có bắt buộc phải tip không?</t>
   </si>
   <si>
-    <t>It’s not required, but appreciated.</t>
-  </si>
-  <si>
     <t>/ɪts nɑt rɪˈkwaɪrd, bʌt əˈpriʃiˌeɪtɪd/</t>
   </si>
   <si>
@@ -1056,9 +984,6 @@
     <t>/kæn ju hɛlp mi, pliz?/</t>
   </si>
   <si>
-    <t>Yes, what’s wrong?</t>
-  </si>
-  <si>
     <t>/jɛs, wʌts rɔŋ?/</t>
   </si>
   <si>
@@ -1122,9 +1047,6 @@
     <t>Ai đó đã lấy trộm túi của tôi!</t>
   </si>
   <si>
-    <t>Let’s call security.</t>
-  </si>
-  <si>
     <t>/lɛts kɔl sɪˈkjʊrɪti/</t>
   </si>
   <si>
@@ -1140,9 +1062,6 @@
     <t>Tôi cần xe cứu thương!</t>
   </si>
   <si>
-    <t>I’ll call 911 right now!</t>
-  </si>
-  <si>
     <t>/aɪl kɔl ˌnaɪn wʌn wʌn raɪt naʊ!/</t>
   </si>
   <si>
@@ -1158,9 +1077,6 @@
     <t>Bạn tôi bất tỉnh rồi!</t>
   </si>
   <si>
-    <t>Stay calm, I’ll get help!</t>
-  </si>
-  <si>
     <t>/steɪ kɑm, aɪl gɛt hɛlp!/</t>
   </si>
   <si>
@@ -1176,9 +1092,6 @@
     <t>Có hiệu thuốc nào gần đây không?</t>
   </si>
   <si>
-    <t>Yes, there’s one around the corner.</t>
-  </si>
-  <si>
     <t>/jɛs, ðɛrz wʌn əˈraʊnd ðə ˈkɔrnɚ/</t>
   </si>
   <si>
@@ -1212,9 +1125,6 @@
     <t>Lối thoát hiểm ở đâu?</t>
   </si>
   <si>
-    <t>It’s at the end of the hallway.</t>
-  </si>
-  <si>
     <t>/ɪts æt ði ɛnd ʌv ðə ˈhɔlweɪ/</t>
   </si>
   <si>
@@ -1224,9 +1134,6 @@
     <t>Cái này giá bao nhiêu?</t>
   </si>
   <si>
-    <t>It’s $25.</t>
-  </si>
-  <si>
     <t>/ɪts twɛnti faɪv dɑlərz/</t>
   </si>
   <si>
@@ -1281,9 +1188,6 @@
     <t>Món này có giảm giá không?</t>
   </si>
   <si>
-    <t>Yes, it’s 20% off today.</t>
-  </si>
-  <si>
     <t>/jɛs, ɪts twɛnti pɚsɛnt ɔf təˈdeɪ/</t>
   </si>
   <si>
@@ -1359,9 +1263,6 @@
     <t>Giờ mở cửa của cửa hàng là gì?</t>
   </si>
   <si>
-    <t>We’re open from 9 AM to 9 PM.</t>
-  </si>
-  <si>
     <t>/wɪr ˈoʊpən frʌm naɪn eɪ ɛm tu naɪn pi ɛm/</t>
   </si>
   <si>
@@ -1398,9 +1299,6 @@
     <t>Một phòng một đêm giá bao nhiêu?</t>
   </si>
   <si>
-    <t>It’s $80 per night.</t>
-  </si>
-  <si>
     <t>/ɪts ˈeɪti dɑlərz pɝ naɪt/</t>
   </si>
   <si>
@@ -1452,9 +1350,6 @@
     <t>Tôi có thể thuê xe ở đâu?</t>
   </si>
   <si>
-    <t>There’s a rental service nearby.</t>
-  </si>
-  <si>
     <t>/ðɛrz ə ˈrɛntəl ˈsɝvɪs ˌnɪrˈbaɪ/</t>
   </si>
   <si>
@@ -1479,18 +1374,12 @@
     <t>Ở đây có phương tiện công cộng không?</t>
   </si>
   <si>
-    <t>Yes, there’s a subway nearby.</t>
-  </si>
-  <si>
     <t>/jɛs, ðɛrz ə ˈsʌbweɪ ˌnɪrˈbaɪ/</t>
   </si>
   <si>
     <t>Có, có tàu điện ngầm gần đây.</t>
   </si>
   <si>
-    <t>There’s a currency exchange at the mall.</t>
-  </si>
-  <si>
     <t>/ðɛrz ə ˈkɝrənsi ɪksˈʧeɪndʒ æt ðə mɔl/</t>
   </si>
   <si>
@@ -1551,9 +1440,6 @@
     <t>Bạn có bị dị ứng gì không?</t>
   </si>
   <si>
-    <t>No, I don’t have any.</t>
-  </si>
-  <si>
     <t>/noʊ, aɪ doʊnt hæv ˈɛni/</t>
   </si>
   <si>
@@ -1587,9 +1473,6 @@
     <t>Bạn có thể mô tả cơn đau không?</t>
   </si>
   <si>
-    <t>It’s a sharp pain in my stomach.</t>
-  </si>
-  <si>
     <t>/ɪts ə ʃɑrp peɪn ɪn maɪ ˈstʌmək/</t>
   </si>
   <si>
@@ -1605,9 +1488,6 @@
     <t>Tôi có cần đơn thuốc cho cái này không?</t>
   </si>
   <si>
-    <t>Yes, you need a doctor’s prescription.</t>
-  </si>
-  <si>
     <t>/jɛs, jʊ nid ə ˈdɑktɚz prɪˈskrɪpʃən/</t>
   </si>
   <si>
@@ -1684,6 +1564,126 @@
   </si>
   <si>
     <t>Ăn nhẹ, thực phẩm bổ dưỡng và uống nhiều nước.</t>
+  </si>
+  <si>
+    <t>How's it going?</t>
+  </si>
+  <si>
+    <t>What's up?</t>
+  </si>
+  <si>
+    <t>Yeah, what's up?</t>
+  </si>
+  <si>
+    <t>I'm from New York.</t>
+  </si>
+  <si>
+    <t>I'm a teacher.</t>
+  </si>
+  <si>
+    <t>Yeah, it's nice!</t>
+  </si>
+  <si>
+    <t>It's 3 PM.</t>
+  </si>
+  <si>
+    <t>No, it's separate.</t>
+  </si>
+  <si>
+    <t>It's $25.99.</t>
+  </si>
+  <si>
+    <t>Can I return this if it doesn't fit?</t>
+  </si>
+  <si>
+    <t>What's your return policy?</t>
+  </si>
+  <si>
+    <t>It's two blocks away.</t>
+  </si>
+  <si>
+    <t>What's the best way to get around?</t>
+  </si>
+  <si>
+    <t>It's $10 per person.</t>
+  </si>
+  <si>
+    <t>Sure! I'm Alex, a project manager.</t>
+  </si>
+  <si>
+    <t>It's due next Friday.</t>
+  </si>
+  <si>
+    <t>You'll report to the department manager.</t>
+  </si>
+  <si>
+    <t>They're on the company's shared drive.</t>
+  </si>
+  <si>
+    <t>What's the next step in this process?</t>
+  </si>
+  <si>
+    <t>Sure, I'll email it to you now.</t>
+  </si>
+  <si>
+    <t>How was the client's feedback?</t>
+  </si>
+  <si>
+    <t>Of course! I'll bring it right away.</t>
+  </si>
+  <si>
+    <t>Sure! I'll bring one for you.</t>
+  </si>
+  <si>
+    <t>It's not required, but appreciated.</t>
+  </si>
+  <si>
+    <t>Yes, what's wrong?</t>
+  </si>
+  <si>
+    <t>Let's call security.</t>
+  </si>
+  <si>
+    <t>I'll call 911 right now!</t>
+  </si>
+  <si>
+    <t>Stay calm, I'll get help!</t>
+  </si>
+  <si>
+    <t>Yes, there's one around the corner.</t>
+  </si>
+  <si>
+    <t>It's at the end of the hallway.</t>
+  </si>
+  <si>
+    <t>It's $25.</t>
+  </si>
+  <si>
+    <t>Yes, it's 20% off today.</t>
+  </si>
+  <si>
+    <t>We're open from 9 AM to 9 PM.</t>
+  </si>
+  <si>
+    <t>It's $80 per night.</t>
+  </si>
+  <si>
+    <t>There's a rental service nearby.</t>
+  </si>
+  <si>
+    <t>Yes, there's a subway nearby.</t>
+  </si>
+  <si>
+    <t>There's a currency exchange at the mall.</t>
+  </si>
+  <si>
+    <t>No, I don't have any.</t>
+  </si>
+  <si>
+    <t>It's a sharp pain in my stomach.</t>
+  </si>
+  <si>
+    <t>Yes, you need a doctor's prescription.</t>
   </si>
 </sst>
 </file>
@@ -1736,6 +1736,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2003,13 +2007,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2018,19 +2022,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G1">
         <v>1</v>
@@ -2038,22 +2042,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" t="s">
-        <v>83</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2061,22 +2065,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>514</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2084,22 +2088,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2107,22 +2111,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2130,22 +2134,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>515</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2156,19 +2160,19 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
+        <v>516</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
         <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -2176,22 +2180,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -2199,22 +2203,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>517</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s">
         <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -2222,22 +2226,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>518</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2245,22 +2249,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>519</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -2268,22 +2272,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -2291,22 +2295,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -2314,22 +2318,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -2337,22 +2341,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -2360,22 +2364,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
         <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -2383,22 +2387,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -2406,22 +2410,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
         <v>56</v>
-      </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" t="s">
-        <v>59</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -2429,22 +2433,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
         <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" t="s">
-        <v>65</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -2452,22 +2456,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>520</v>
+      </c>
+      <c r="E20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" t="s">
+      <c r="F20" t="s">
         <v>67</v>
-      </c>
-      <c r="C20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" t="s">
-        <v>71</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -2475,22 +2479,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="F21" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" t="s">
-        <v>77</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -2498,22 +2502,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G22">
         <v>3</v>
@@ -2521,22 +2525,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>521</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G23">
         <v>3</v>
@@ -2544,22 +2548,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G24">
         <v>3</v>
@@ -2567,22 +2571,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G25">
         <v>3</v>
@@ -2590,22 +2594,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F26" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G26">
         <v>3</v>
@@ -2613,22 +2617,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G27">
         <v>3</v>
@@ -2636,22 +2640,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>522</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G28">
         <v>3</v>
@@ -2659,22 +2663,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D29" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E29" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F29" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G29">
         <v>3</v>
@@ -2682,22 +2686,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C30" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F30" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G30">
         <v>3</v>
@@ -2705,22 +2709,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>523</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D31" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E31" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F31" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="G31">
         <v>3</v>
@@ -2728,22 +2732,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>524</v>
       </c>
       <c r="E32" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F32" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="G32">
         <v>4</v>
@@ -2751,22 +2755,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D33" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E33" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="G33">
         <v>4</v>
@@ -2774,22 +2778,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>525</v>
       </c>
       <c r="B34" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="D34" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="E34" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F34" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="G34">
         <v>4</v>
@@ -2797,22 +2801,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="D35" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E35" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="F35" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="G35">
         <v>4</v>
@@ -2820,22 +2824,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C36" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="D36" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E36" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="F36" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="G36">
         <v>4</v>
@@ -2843,22 +2847,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C37" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D37" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="E37" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="F37" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="G37">
         <v>4</v>
@@ -2866,22 +2870,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B38" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D38" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="E38" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="F38" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="G38">
         <v>4</v>
@@ -2889,22 +2893,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B39" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C39" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D39" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="E39" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F39" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="G39">
         <v>4</v>
@@ -2912,22 +2916,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C40" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D40" t="s">
-        <v>233</v>
+        <v>526</v>
       </c>
       <c r="E40" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F40" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="G40">
         <v>4</v>
@@ -2935,22 +2939,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B41" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C41" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="D41" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="E41" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="F41" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G41">
         <v>4</v>
@@ -2958,22 +2962,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B42" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C42" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="D42" t="s">
-        <v>245</v>
+        <v>527</v>
       </c>
       <c r="E42" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="F42" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G42">
         <v>5</v>
@@ -2981,22 +2985,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B43" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="D43" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E43" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="F43" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -3004,22 +3008,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C44" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="D44" t="s">
-        <v>257</v>
+        <v>528</v>
       </c>
       <c r="E44" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="F44" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="G44">
         <v>5</v>
@@ -3027,22 +3031,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B45" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D45" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="E45" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="F45" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -3050,22 +3054,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B46" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="C46" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="D46" t="s">
-        <v>269</v>
+        <v>529</v>
       </c>
       <c r="E46" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="F46" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -3073,22 +3077,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B47" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C47" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="D47" t="s">
-        <v>275</v>
+        <v>530</v>
       </c>
       <c r="E47" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="F47" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="G47">
         <v>5</v>
@@ -3096,22 +3100,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="C48" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="D48" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="E48" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="F48" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="G48">
         <v>5</v>
@@ -3119,22 +3123,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>284</v>
+        <v>531</v>
       </c>
       <c r="B49" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="C49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="D49" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="E49" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="F49" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="G49">
         <v>5</v>
@@ -3142,22 +3146,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="B50" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="C50" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="D50" t="s">
-        <v>293</v>
+        <v>532</v>
       </c>
       <c r="E50" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="F50" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="G50">
         <v>5</v>
@@ -3165,22 +3169,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>296</v>
+        <v>533</v>
       </c>
       <c r="B51" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="C51" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="D51" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="E51" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="F51" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="G51">
         <v>5</v>
@@ -3188,22 +3192,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
         <v>18</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
         <v>19</v>
       </c>
-      <c r="C52" t="s">
+      <c r="F52" t="s">
         <v>20</v>
-      </c>
-      <c r="D52" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" t="s">
-        <v>23</v>
       </c>
       <c r="G52">
         <v>6</v>
@@ -3211,22 +3215,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B53" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="C53" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="E53" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="F53" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G53">
         <v>6</v>
@@ -3234,22 +3238,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
         <v>30</v>
       </c>
-      <c r="B54" t="s">
+      <c r="E54" t="s">
         <v>31</v>
       </c>
-      <c r="C54" t="s">
+      <c r="F54" t="s">
         <v>32</v>
-      </c>
-      <c r="D54" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" t="s">
-        <v>35</v>
       </c>
       <c r="G54">
         <v>6</v>
@@ -3257,22 +3261,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="B55" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="C55" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="D55" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="E55" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="F55" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="G55">
         <v>6</v>
@@ -3280,22 +3284,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="B56" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C56" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="D56" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="E56" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="F56" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="G56">
         <v>6</v>
@@ -3303,22 +3307,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="B57" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="C57" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E57" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="F57" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G57">
         <v>6</v>
@@ -3326,22 +3330,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="B58" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="C58" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D58" t="s">
-        <v>324</v>
+        <v>534</v>
       </c>
       <c r="E58" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="F58" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="G58">
         <v>6</v>
@@ -3349,22 +3353,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C59" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="D59" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="E59" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="F59" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="G59">
         <v>6</v>
@@ -3372,22 +3376,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>332</v>
+        <v>535</v>
       </c>
       <c r="E60" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="F60" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="G60">
         <v>6</v>
@@ -3395,22 +3399,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="B61" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="C61" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="D61" t="s">
-        <v>338</v>
+        <v>536</v>
       </c>
       <c r="E61" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="F61" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="G61">
         <v>6</v>
@@ -3418,22 +3422,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="B62" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>343</v>
+        <v>537</v>
       </c>
       <c r="E62" t="s">
-        <v>344</v>
+        <v>319</v>
       </c>
       <c r="F62" t="s">
-        <v>345</v>
+        <v>320</v>
       </c>
       <c r="G62">
         <v>7</v>
@@ -3441,22 +3445,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="B63" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C63" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="D63" t="s">
-        <v>349</v>
+        <v>324</v>
       </c>
       <c r="E63" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="F63" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="G63">
         <v>7</v>
@@ -3464,22 +3468,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="B64" t="s">
-        <v>353</v>
+        <v>328</v>
       </c>
       <c r="C64" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="D64" t="s">
-        <v>185</v>
+        <v>524</v>
       </c>
       <c r="E64" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F64" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="G64">
         <v>7</v>
@@ -3487,22 +3491,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="B65" t="s">
-        <v>357</v>
+        <v>332</v>
       </c>
       <c r="C65" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="D65" t="s">
-        <v>359</v>
+        <v>334</v>
       </c>
       <c r="E65" t="s">
-        <v>360</v>
+        <v>335</v>
       </c>
       <c r="F65" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="G65">
         <v>7</v>
@@ -3510,22 +3514,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="B66" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="C66" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="D66" t="s">
-        <v>365</v>
+        <v>538</v>
       </c>
       <c r="E66" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="F66" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="G66">
         <v>7</v>
@@ -3533,22 +3537,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="B67" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="C67" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
       <c r="D67" t="s">
-        <v>371</v>
+        <v>539</v>
       </c>
       <c r="E67" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="F67" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="G67">
         <v>7</v>
@@ -3556,22 +3560,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="B68" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="C68" t="s">
-        <v>376</v>
+        <v>349</v>
       </c>
       <c r="D68" t="s">
-        <v>377</v>
+        <v>540</v>
       </c>
       <c r="E68" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="F68" t="s">
-        <v>379</v>
+        <v>351</v>
       </c>
       <c r="G68">
         <v>7</v>
@@ -3579,22 +3583,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
       <c r="B69" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
       <c r="C69" t="s">
-        <v>382</v>
+        <v>354</v>
       </c>
       <c r="D69" t="s">
-        <v>383</v>
+        <v>541</v>
       </c>
       <c r="E69" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="F69" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
       <c r="G69">
         <v>7</v>
@@ -3602,22 +3606,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>386</v>
+        <v>357</v>
       </c>
       <c r="B70" t="s">
-        <v>387</v>
+        <v>358</v>
       </c>
       <c r="C70" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="D70" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="E70" t="s">
-        <v>390</v>
+        <v>361</v>
       </c>
       <c r="F70" t="s">
-        <v>391</v>
+        <v>362</v>
       </c>
       <c r="G70">
         <v>7</v>
@@ -3625,22 +3629,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>392</v>
+        <v>363</v>
       </c>
       <c r="B71" t="s">
-        <v>393</v>
+        <v>364</v>
       </c>
       <c r="C71" t="s">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="D71" t="s">
-        <v>395</v>
+        <v>542</v>
       </c>
       <c r="E71" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
       <c r="F71" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
       <c r="G71">
         <v>7</v>
@@ -3648,22 +3652,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C72" t="s">
-        <v>398</v>
+        <v>368</v>
       </c>
       <c r="D72" t="s">
-        <v>399</v>
+        <v>543</v>
       </c>
       <c r="E72" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="F72" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="G72">
         <v>8</v>
@@ -3671,22 +3675,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="B73" t="s">
-        <v>403</v>
+        <v>372</v>
       </c>
       <c r="C73" t="s">
-        <v>404</v>
+        <v>373</v>
       </c>
       <c r="D73" t="s">
-        <v>405</v>
+        <v>374</v>
       </c>
       <c r="E73" t="s">
-        <v>406</v>
+        <v>375</v>
       </c>
       <c r="F73" t="s">
-        <v>407</v>
+        <v>376</v>
       </c>
       <c r="G73">
         <v>8</v>
@@ -3694,22 +3698,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>408</v>
+        <v>377</v>
       </c>
       <c r="D74" t="s">
-        <v>409</v>
+        <v>378</v>
       </c>
       <c r="E74" t="s">
-        <v>410</v>
+        <v>379</v>
       </c>
       <c r="F74" t="s">
-        <v>411</v>
+        <v>380</v>
       </c>
       <c r="G74">
         <v>8</v>
@@ -3717,22 +3721,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>412</v>
+        <v>381</v>
       </c>
       <c r="B75" t="s">
-        <v>413</v>
+        <v>382</v>
       </c>
       <c r="C75" t="s">
-        <v>414</v>
+        <v>383</v>
       </c>
       <c r="D75" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E75" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F75" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G75">
         <v>8</v>
@@ -3740,22 +3744,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="B76" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
       <c r="C76" t="s">
-        <v>417</v>
+        <v>386</v>
       </c>
       <c r="D76" t="s">
-        <v>418</v>
+        <v>544</v>
       </c>
       <c r="E76" t="s">
-        <v>419</v>
+        <v>387</v>
       </c>
       <c r="F76" t="s">
-        <v>420</v>
+        <v>388</v>
       </c>
       <c r="G76">
         <v>8</v>
@@ -3763,22 +3767,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>421</v>
+        <v>389</v>
       </c>
       <c r="B77" t="s">
-        <v>422</v>
+        <v>390</v>
       </c>
       <c r="C77" t="s">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="D77" t="s">
-        <v>424</v>
+        <v>392</v>
       </c>
       <c r="E77" t="s">
-        <v>425</v>
+        <v>393</v>
       </c>
       <c r="F77" t="s">
-        <v>426</v>
+        <v>394</v>
       </c>
       <c r="G77">
         <v>8</v>
@@ -3786,22 +3790,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>522</v>
       </c>
       <c r="B78" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="C78" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D78" t="s">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="E78" t="s">
-        <v>429</v>
+        <v>397</v>
       </c>
       <c r="F78" t="s">
-        <v>430</v>
+        <v>398</v>
       </c>
       <c r="G78">
         <v>8</v>
@@ -3809,22 +3813,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>431</v>
+        <v>399</v>
       </c>
       <c r="B79" t="s">
-        <v>432</v>
+        <v>400</v>
       </c>
       <c r="C79" t="s">
-        <v>433</v>
+        <v>401</v>
       </c>
       <c r="D79" t="s">
-        <v>434</v>
+        <v>402</v>
       </c>
       <c r="E79" t="s">
-        <v>435</v>
+        <v>403</v>
       </c>
       <c r="F79" t="s">
-        <v>436</v>
+        <v>404</v>
       </c>
       <c r="G79">
         <v>8</v>
@@ -3832,22 +3836,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>437</v>
+        <v>405</v>
       </c>
       <c r="B80" t="s">
-        <v>438</v>
+        <v>406</v>
       </c>
       <c r="C80" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D80" t="s">
-        <v>439</v>
+        <v>407</v>
       </c>
       <c r="E80" t="s">
-        <v>440</v>
+        <v>408</v>
       </c>
       <c r="F80" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G80">
         <v>8</v>
@@ -3855,22 +3859,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>441</v>
+        <v>409</v>
       </c>
       <c r="B81" t="s">
-        <v>442</v>
+        <v>410</v>
       </c>
       <c r="C81" t="s">
-        <v>443</v>
+        <v>411</v>
       </c>
       <c r="D81" t="s">
-        <v>444</v>
+        <v>545</v>
       </c>
       <c r="E81" t="s">
-        <v>445</v>
+        <v>412</v>
       </c>
       <c r="F81" t="s">
-        <v>446</v>
+        <v>413</v>
       </c>
       <c r="G81">
         <v>8</v>
@@ -3878,22 +3882,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B82" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C82" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D82" t="s">
-        <v>185</v>
+        <v>524</v>
       </c>
       <c r="E82" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F82" t="s">
-        <v>447</v>
+        <v>414</v>
       </c>
       <c r="G82">
         <v>9</v>
@@ -3901,22 +3905,22 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>448</v>
+        <v>415</v>
       </c>
       <c r="B83" t="s">
-        <v>449</v>
+        <v>416</v>
       </c>
       <c r="C83" t="s">
-        <v>450</v>
+        <v>417</v>
       </c>
       <c r="D83" t="s">
-        <v>451</v>
+        <v>418</v>
       </c>
       <c r="E83" t="s">
-        <v>452</v>
+        <v>419</v>
       </c>
       <c r="F83" t="s">
-        <v>453</v>
+        <v>420</v>
       </c>
       <c r="G83">
         <v>9</v>
@@ -3924,22 +3928,22 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>454</v>
+        <v>421</v>
       </c>
       <c r="B84" t="s">
-        <v>455</v>
+        <v>422</v>
       </c>
       <c r="C84" t="s">
-        <v>456</v>
+        <v>423</v>
       </c>
       <c r="D84" t="s">
-        <v>457</v>
+        <v>546</v>
       </c>
       <c r="E84" t="s">
-        <v>458</v>
+        <v>424</v>
       </c>
       <c r="F84" t="s">
-        <v>459</v>
+        <v>425</v>
       </c>
       <c r="G84">
         <v>9</v>
@@ -3947,22 +3951,22 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>460</v>
+        <v>426</v>
       </c>
       <c r="B85" t="s">
-        <v>461</v>
+        <v>427</v>
       </c>
       <c r="C85" t="s">
-        <v>462</v>
+        <v>428</v>
       </c>
       <c r="D85" t="s">
-        <v>463</v>
+        <v>429</v>
       </c>
       <c r="E85" t="s">
-        <v>464</v>
+        <v>430</v>
       </c>
       <c r="F85" t="s">
-        <v>465</v>
+        <v>431</v>
       </c>
       <c r="G85">
         <v>9</v>
@@ -3970,22 +3974,22 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>466</v>
+        <v>432</v>
       </c>
       <c r="B86" t="s">
-        <v>467</v>
+        <v>433</v>
       </c>
       <c r="C86" t="s">
-        <v>468</v>
+        <v>434</v>
       </c>
       <c r="D86" t="s">
-        <v>469</v>
+        <v>435</v>
       </c>
       <c r="E86" t="s">
-        <v>470</v>
+        <v>436</v>
       </c>
       <c r="F86" t="s">
-        <v>471</v>
+        <v>437</v>
       </c>
       <c r="G86">
         <v>9</v>
@@ -3993,22 +3997,22 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>472</v>
+        <v>438</v>
       </c>
       <c r="B87" t="s">
-        <v>473</v>
+        <v>439</v>
       </c>
       <c r="C87" t="s">
-        <v>474</v>
+        <v>440</v>
       </c>
       <c r="D87" t="s">
-        <v>475</v>
+        <v>547</v>
       </c>
       <c r="E87" t="s">
-        <v>476</v>
+        <v>441</v>
       </c>
       <c r="F87" t="s">
-        <v>477</v>
+        <v>442</v>
       </c>
       <c r="G87">
         <v>9</v>
@@ -4016,22 +4020,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
-        <v>478</v>
+        <v>443</v>
       </c>
       <c r="C88" t="s">
-        <v>479</v>
+        <v>444</v>
       </c>
       <c r="D88" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E88" t="s">
-        <v>480</v>
+        <v>445</v>
       </c>
       <c r="F88" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="G88">
         <v>9</v>
@@ -4039,22 +4043,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>481</v>
+        <v>446</v>
       </c>
       <c r="B89" t="s">
-        <v>482</v>
+        <v>447</v>
       </c>
       <c r="C89" t="s">
-        <v>483</v>
+        <v>448</v>
       </c>
       <c r="D89" t="s">
-        <v>484</v>
+        <v>548</v>
       </c>
       <c r="E89" t="s">
-        <v>485</v>
+        <v>449</v>
       </c>
       <c r="F89" t="s">
-        <v>486</v>
+        <v>450</v>
       </c>
       <c r="G89">
         <v>9</v>
@@ -4062,22 +4066,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B90" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C90" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D90" t="s">
-        <v>487</v>
+        <v>549</v>
       </c>
       <c r="E90" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="F90" t="s">
-        <v>489</v>
+        <v>452</v>
       </c>
       <c r="G90">
         <v>9</v>
@@ -4085,22 +4089,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B91" t="s">
-        <v>490</v>
+        <v>453</v>
       </c>
       <c r="C91" t="s">
-        <v>491</v>
+        <v>454</v>
       </c>
       <c r="D91" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E91" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="F91" t="s">
-        <v>492</v>
+        <v>455</v>
       </c>
       <c r="G91">
         <v>9</v>
@@ -4108,22 +4112,22 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>493</v>
+        <v>456</v>
       </c>
       <c r="B92" t="s">
-        <v>494</v>
+        <v>457</v>
       </c>
       <c r="C92" t="s">
-        <v>495</v>
+        <v>458</v>
       </c>
       <c r="D92" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="E92" t="s">
-        <v>497</v>
+        <v>460</v>
       </c>
       <c r="F92" t="s">
-        <v>498</v>
+        <v>461</v>
       </c>
       <c r="G92">
         <v>10</v>
@@ -4131,22 +4135,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>499</v>
+        <v>462</v>
       </c>
       <c r="B93" t="s">
-        <v>500</v>
+        <v>463</v>
       </c>
       <c r="C93" t="s">
-        <v>501</v>
+        <v>464</v>
       </c>
       <c r="D93" t="s">
-        <v>502</v>
+        <v>465</v>
       </c>
       <c r="E93" t="s">
-        <v>503</v>
+        <v>466</v>
       </c>
       <c r="F93" t="s">
-        <v>504</v>
+        <v>467</v>
       </c>
       <c r="G93">
         <v>10</v>
@@ -4154,22 +4158,22 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>505</v>
+        <v>468</v>
       </c>
       <c r="B94" t="s">
-        <v>506</v>
+        <v>469</v>
       </c>
       <c r="C94" t="s">
-        <v>507</v>
+        <v>470</v>
       </c>
       <c r="D94" t="s">
-        <v>508</v>
+        <v>550</v>
       </c>
       <c r="E94" t="s">
-        <v>509</v>
+        <v>471</v>
       </c>
       <c r="F94" t="s">
-        <v>510</v>
+        <v>472</v>
       </c>
       <c r="G94">
         <v>10</v>
@@ -4177,22 +4181,22 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>511</v>
+        <v>473</v>
       </c>
       <c r="B95" t="s">
-        <v>512</v>
+        <v>474</v>
       </c>
       <c r="C95" t="s">
-        <v>513</v>
+        <v>475</v>
       </c>
       <c r="D95" t="s">
-        <v>514</v>
+        <v>476</v>
       </c>
       <c r="E95" t="s">
-        <v>515</v>
+        <v>477</v>
       </c>
       <c r="F95" t="s">
-        <v>516</v>
+        <v>478</v>
       </c>
       <c r="G95">
         <v>10</v>
@@ -4200,22 +4204,22 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>517</v>
+        <v>479</v>
       </c>
       <c r="B96" t="s">
-        <v>518</v>
+        <v>480</v>
       </c>
       <c r="C96" t="s">
-        <v>519</v>
+        <v>481</v>
       </c>
       <c r="D96" t="s">
-        <v>520</v>
+        <v>551</v>
       </c>
       <c r="E96" t="s">
-        <v>521</v>
+        <v>482</v>
       </c>
       <c r="F96" t="s">
-        <v>522</v>
+        <v>483</v>
       </c>
       <c r="G96">
         <v>10</v>
@@ -4223,22 +4227,22 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>523</v>
+        <v>484</v>
       </c>
       <c r="B97" t="s">
-        <v>524</v>
+        <v>485</v>
       </c>
       <c r="C97" t="s">
-        <v>525</v>
+        <v>486</v>
       </c>
       <c r="D97" t="s">
-        <v>526</v>
+        <v>552</v>
       </c>
       <c r="E97" t="s">
-        <v>527</v>
+        <v>487</v>
       </c>
       <c r="F97" t="s">
-        <v>528</v>
+        <v>488</v>
       </c>
       <c r="G97">
         <v>10</v>
@@ -4246,22 +4250,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>529</v>
+        <v>489</v>
       </c>
       <c r="B98" t="s">
-        <v>530</v>
+        <v>490</v>
       </c>
       <c r="C98" t="s">
-        <v>531</v>
+        <v>491</v>
       </c>
       <c r="D98" t="s">
-        <v>532</v>
+        <v>492</v>
       </c>
       <c r="E98" t="s">
-        <v>533</v>
+        <v>493</v>
       </c>
       <c r="F98" t="s">
-        <v>534</v>
+        <v>494</v>
       </c>
       <c r="G98">
         <v>10</v>
@@ -4269,22 +4273,22 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>535</v>
+        <v>495</v>
       </c>
       <c r="B99" t="s">
-        <v>536</v>
+        <v>496</v>
       </c>
       <c r="C99" t="s">
-        <v>537</v>
+        <v>497</v>
       </c>
       <c r="D99" t="s">
-        <v>538</v>
+        <v>498</v>
       </c>
       <c r="E99" t="s">
-        <v>539</v>
+        <v>499</v>
       </c>
       <c r="F99" t="s">
-        <v>540</v>
+        <v>500</v>
       </c>
       <c r="G99">
         <v>10</v>
@@ -4292,22 +4296,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>541</v>
+        <v>501</v>
       </c>
       <c r="B100" t="s">
-        <v>542</v>
+        <v>502</v>
       </c>
       <c r="C100" t="s">
-        <v>543</v>
+        <v>503</v>
       </c>
       <c r="D100" t="s">
-        <v>544</v>
+        <v>504</v>
       </c>
       <c r="E100" t="s">
-        <v>545</v>
+        <v>505</v>
       </c>
       <c r="F100" t="s">
-        <v>546</v>
+        <v>506</v>
       </c>
       <c r="G100">
         <v>10</v>
@@ -4315,22 +4319,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>547</v>
+        <v>507</v>
       </c>
       <c r="B101" t="s">
-        <v>548</v>
+        <v>508</v>
       </c>
       <c r="C101" t="s">
-        <v>549</v>
+        <v>509</v>
       </c>
       <c r="D101" t="s">
-        <v>550</v>
+        <v>510</v>
       </c>
       <c r="E101" t="s">
-        <v>551</v>
+        <v>511</v>
       </c>
       <c r="F101" t="s">
-        <v>552</v>
+        <v>512</v>
       </c>
       <c r="G101">
         <v>10</v>

</xml_diff>